<commit_message>
updates to additional species and rerun interactive figure
</commit_message>
<xml_diff>
--- a/data/additional-species.xlsx
+++ b/data/additional-species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MANUSCRIPTS WORKING ON\Allometry of breating frequency\Stats\Stacy-revised analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sld33/Dropbox/mammal-breath-rate/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4AEEB2-8590-4633-8FCD-F5BAE1BA810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF54BEAE-C967-1946-B397-CD3A6DACA244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="98" yWindow="585" windowWidth="11707" windowHeight="10140" xr2:uid="{10BD9EF6-2208-4254-B9C3-01D5A8855853}"/>
+    <workbookView xWindow="-12260" yWindow="-1640" windowWidth="11700" windowHeight="10140" xr2:uid="{10BD9EF6-2208-4254-B9C3-01D5A8855853}"/>
   </bookViews>
   <sheets>
     <sheet name="mortola" sheetId="1" r:id="rId1"/>
@@ -143,18 +143,12 @@
     <t>Capybara</t>
   </si>
   <si>
-    <t>False killwe whale</t>
-  </si>
-  <si>
     <t>Amazonian manatee</t>
   </si>
   <si>
     <t>Antarctic fur seal</t>
   </si>
   <si>
-    <t>California Sea Lions</t>
-  </si>
-  <si>
     <t>Beaver</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>Dugon</t>
+  </si>
+  <si>
+    <t>False killer whale</t>
+  </si>
+  <si>
+    <t>California Sea Lion</t>
   </si>
 </sst>
 </file>
@@ -549,13 +549,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD151AC-824A-4550-8434-C55E1597C8E3}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1135</v>
       </c>
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>159</v>
       </c>
@@ -606,7 +606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>52</v>
       </c>
@@ -623,7 +623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6650</v>
       </c>
@@ -640,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2883</v>
       </c>
@@ -657,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1034</v>
       </c>
@@ -674,7 +674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3842.5</v>
       </c>
@@ -691,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>51700</v>
       </c>
@@ -708,7 +708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>200</v>
       </c>
@@ -725,7 +725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>77</v>
       </c>
@@ -742,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>70</v>
       </c>
@@ -759,7 +759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>72</v>
       </c>
@@ -776,7 +776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>206</v>
       </c>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1175</v>
       </c>
@@ -810,7 +810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>283</v>
       </c>
@@ -827,7 +827,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>190</v>
       </c>
@@ -844,7 +844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>425</v>
       </c>
@@ -861,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>227</v>
       </c>
@@ -878,7 +878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1700</v>
       </c>
@@ -895,7 +895,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>310</v>
       </c>
@@ -912,7 +912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -929,7 +929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -946,7 +946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -957,14 +957,14 @@
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>53</v>
       </c>
@@ -981,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>89</v>
       </c>
@@ -992,13 +992,13 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>360</v>
       </c>
@@ -1009,13 +1009,13 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>275</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -1041,13 +1041,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DE0453-1B1F-4FEE-9306-874EEE86E810}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1115,9 +1115,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>100</v>
@@ -1133,7 +1133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1151,9 +1151,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>77.900000000000006</v>
@@ -1169,7 +1169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>845</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" ref="C10:C17" si="1">LOG10(B10)</f>
+        <f t="shared" ref="C10:C12" si="1">LOG10(B10)</f>
         <v>2.9268567089496922</v>
       </c>
       <c r="D10">
@@ -1223,9 +1223,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>525</v>
@@ -1241,7 +1241,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1259,9 +1259,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -1277,9 +1277,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>250</v>
@@ -1295,9 +1295,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>360</v>

</xml_diff>